<commit_message>
clase jueves 17 agosto
</commit_message>
<xml_diff>
--- a/Machine Learning II/Clase_a_Clase_Machine_Learning_II.xlsx
+++ b/Machine Learning II/Clase_a_Clase_Machine_Learning_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46b6423b4a08acb9/Escritorio/UDLA Mg DS/Machine Learning II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{B9566F63-6B0C-4D28-9508-EFCB0C4A59F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14A3C4F2-1C65-4286-AA0B-8E2C781B9B18}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{B9566F63-6B0C-4D28-9508-EFCB0C4A59F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423EB151-8291-44DD-88FD-8E25D0A1C8E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Fecha</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>1 h rec</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sugerencias: entregar prueba antes del 2/9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fecha entrega maxima: 4/5? </t>
   </si>
 </sst>
 </file>
@@ -311,7 +320,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -368,6 +377,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -670,7 +683,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +695,7 @@
     <col min="5" max="5" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>45113</v>
       </c>
@@ -710,7 +723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>45115</v>
       </c>
@@ -721,7 +734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>45120</v>
       </c>
@@ -732,7 +745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>45122</v>
       </c>
@@ -743,7 +756,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>45127</v>
       </c>
@@ -754,7 +767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>45129</v>
       </c>
@@ -766,7 +779,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>45134</v>
       </c>
@@ -777,7 +790,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>45136</v>
       </c>
@@ -786,7 +799,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>45141</v>
       </c>
@@ -795,7 +808,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>45143</v>
       </c>
@@ -804,7 +817,7 @@
       </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>45148</v>
       </c>
@@ -816,7 +829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>45150</v>
       </c>
@@ -824,11 +837,8 @@
         <v>12</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>45155</v>
       </c>
@@ -836,11 +846,17 @@
         <v>13</v>
       </c>
       <c r="C14" s="6"/>
+      <c r="D14" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="E14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>45157</v>
       </c>
@@ -857,7 +873,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>45162</v>
       </c>
@@ -918,9 +934,15 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
       <c r="E24" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion excel clase a clase
</commit_message>
<xml_diff>
--- a/Machine Learning II/Clase_a_Clase_Machine_Learning_II.xlsx
+++ b/Machine Learning II/Clase_a_Clase_Machine_Learning_II.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46b6423b4a08acb9/Escritorio/UDLA Mg DS/Machine Learning II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{B9566F63-6B0C-4D28-9508-EFCB0C4A59F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423EB151-8291-44DD-88FD-8E25D0A1C8E4}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{B9566F63-6B0C-4D28-9508-EFCB0C4A59F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{795C39BF-35F8-4335-9739-EEF8F1EDC632}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Fecha</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Desarrollo y producción de modelos de machine learning</t>
-  </si>
-  <si>
-    <t>fecha actual</t>
   </si>
   <si>
     <t>Examen</t>
@@ -147,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,13 +183,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="2" tint="-0.249977111117893"/>
@@ -214,18 +204,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -314,47 +298,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +664,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,220 +680,232 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>45113</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <v>45113</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>45115</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>45120</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>45122</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>45127</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>45129</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>45134</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>45136</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>45141</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>45143</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>45148</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5"/>
       <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>45150</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>45155</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="13">
+        <v>45155</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>45157</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="13">
+        <v>45157</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>45162</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="13">
+        <v>45164</v>
+      </c>
+      <c r="E16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
-        <v>45150</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>45155</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="9" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>45164</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="13">
+        <v>45169</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>45171</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="14">
+        <v>45171</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
         <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>45157</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>45162</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="E16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
-        <v>45164</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="E17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
-        <v>45171</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -935,13 +928,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="3"/>
     </row>

</xml_diff>